<commit_message>
Added SPI Flash ROM
</commit_message>
<xml_diff>
--- a/Eagle/BOM-GD32F103RC.xlsx
+++ b/Eagle/BOM-GD32F103RC.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -52,10 +52,10 @@
     <t xml:space="preserve">C3, C4</t>
   </si>
   <si>
-    <t xml:space="preserve">10pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1634</t>
+    <t xml:space="preserve">12pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C38523</t>
   </si>
   <si>
     <t xml:space="preserve">C5, C6, C13</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">C7171</t>
   </si>
   <si>
-    <t xml:space="preserve">C7, C8, C9, C10, C11, C12, C14, C15, C16, C17</t>
+    <t xml:space="preserve">C7, C8, C9, C10, C11, C12, C14, C15, C16, C17, C18</t>
   </si>
   <si>
     <t xml:space="preserve">100n</t>
@@ -187,16 +187,52 @@
     <t xml:space="preserve">C587158 </t>
   </si>
   <si>
-    <t xml:space="preserve">J3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB_MICRO-B_FEMALE-SMT</t>
+    <t xml:space="preserve">U3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOIC-8_208mil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W25Q128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C97521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10118192-0002LF</t>
   </si>
   <si>
     <t xml:space="preserve">USB-B-MICRO-SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">C404968</t>
+    <t xml:space="preserve">C2972784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HC-49S-SMD-2P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Mhz Crystal 20pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C12674</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FC-12M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32.768kHz Crystal 12.5pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C32346</t>
   </si>
   <si>
     <t xml:space="preserve">SW1, SW2</t>
@@ -301,31 +337,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -402,14 +438,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -418,7 +454,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.58"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -492,7 +528,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -656,7 +692,7 @@
       <c r="D14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="0" t="s">
         <v>50</v>
       </c>
     </row>
@@ -687,34 +723,85 @@
       <c r="C16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="6" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="4" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <f aca="false">SUM(A2:A16)</f>
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <f aca="false">SUM(A2:A20)</f>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>